<commit_message>
fix: Update IMM_AEFI prerelease with missing metadata
</commit_message>
<xml_diff>
--- a/metadata/IMM_AEFI_prerelease/IMM-AEFI_TRACKER_V1_DHIS2.33/reference.xlsx
+++ b/metadata/IMM_AEFI_prerelease/IMM-AEFI_TRACKER_V1_DHIS2.33/reference.xlsx
@@ -22,14 +22,16 @@
     <sheet name="optionGroups" sheetId="17" r:id="rId17"/>
     <sheet name="optionSets" sheetId="18" r:id="rId18"/>
     <sheet name="options" sheetId="19" r:id="rId19"/>
-    <sheet name="dashboards" sheetId="20" r:id="rId20"/>
-    <sheet name="dashboardItems" sheetId="21" r:id="rId21"/>
-    <sheet name="charts" sheetId="22" r:id="rId22"/>
-    <sheet name="maps" sheetId="23" r:id="rId23"/>
-    <sheet name="eventReports" sheetId="24" r:id="rId24"/>
-    <sheet name="programNotificationTemplates" sheetId="25" r:id="rId25"/>
-    <sheet name="userGroups" sheetId="26" r:id="rId26"/>
-    <sheet name="users" sheetId="27" r:id="rId27"/>
+    <sheet name="indicators" sheetId="20" r:id="rId20"/>
+    <sheet name="indicatorTypes" sheetId="21" r:id="rId21"/>
+    <sheet name="dashboards" sheetId="22" r:id="rId22"/>
+    <sheet name="dashboardItems" sheetId="23" r:id="rId23"/>
+    <sheet name="charts" sheetId="24" r:id="rId24"/>
+    <sheet name="maps" sheetId="25" r:id="rId25"/>
+    <sheet name="eventReports" sheetId="26" r:id="rId26"/>
+    <sheet name="programNotificationTemplates" sheetId="27" r:id="rId27"/>
+    <sheet name="userGroups" sheetId="28" r:id="rId28"/>
+    <sheet name="users" sheetId="29" r:id="rId29"/>
   </sheets>
 </workbook>
 </file>
@@ -493,7 +495,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2021-02-16T11:15</v>
+        <v>2021-02-18T03:35</v>
       </c>
     </row>
     <row r="7">
@@ -501,7 +503,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>IMM-AEFI_TRACKER_V1.0.0_DHIS2.33_2021-02-16T11:15</v>
+        <v>IMM-AEFI_TRACKER_V1.0.0_DHIS2.33_2021-02-18T03:35</v>
       </c>
     </row>
   </sheetData>
@@ -550,7 +552,7 @@
         <v>h5FuguPFF2j</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>2020-12-21</v>
+        <v>2021-02-16</v>
       </c>
       <c r="E2" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -567,7 +569,7 @@
         <v>KSr2yTdu1AI</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>2020-12-21</v>
+        <v>2021-02-16</v>
       </c>
       <c r="E3" s="5" t="str">
         <v>EZkN8vYZwjR</v>
@@ -584,7 +586,7 @@
         <v>TfdH5KvFmMy</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>2020-12-21</v>
+        <v>2021-02-16</v>
       </c>
       <c r="E4" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -601,7 +603,7 @@
         <v>aW66s2QSosT</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>2020-12-21</v>
+        <v>2021-02-16</v>
       </c>
       <c r="E5" s="5" t="str">
         <v>EZkN8vYZwjR</v>
@@ -618,7 +620,7 @@
         <v>BiTsLcJQ95V</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>2020-12-21</v>
+        <v>2021-02-16</v>
       </c>
       <c r="E6" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -635,7 +637,7 @@
         <v>CklPZdOd6H1</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>2020-12-21</v>
+        <v>2021-02-16</v>
       </c>
       <c r="E7" s="5" t="str">
         <v>EZkN8vYZwjR</v>
@@ -652,7 +654,7 @@
         <v>VCtm2pySeEV</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>2020-12-21</v>
+        <v>2021-02-16</v>
       </c>
       <c r="E8" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -669,7 +671,7 @@
         <v>pjexi5YaAPa</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>2020-12-21</v>
+        <v>2021-02-16</v>
       </c>
       <c r="E9" s="5" t="str">
         <v>EZkN8vYZwjR</v>
@@ -6526,12 +6528,144 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>UID</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>Shortname</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>Code</v>
+      </c>
+      <c r="E1" s="3" t="str">
+        <v>Description</v>
+      </c>
+      <c r="F1" s="3" t="str">
+        <v>Numerator</v>
+      </c>
+      <c r="G1" s="3" t="str">
+        <v>Denominator</v>
+      </c>
+      <c r="H1" s="3" t="str">
+        <v>Type</v>
+      </c>
+      <c r="I1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="J1" s="3" t="str">
+        <v>Indicator group UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>l1t1lc9JgtS</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>AEFI - Total adverse events reported</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>Total adverse events reported</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E2" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F2" s="4" t="str">
+        <v>Total adverse events</v>
+      </c>
+      <c r="G2" s="4" t="str">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="I2" s="4" t="str">
+        <v>2021-02-05</v>
+      </c>
+      <c r="J2" s="4" t="str">
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Factor</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>2021-01-12</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <v>CqNPn5KzksS</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -6552,7 +6686,7 @@
         <v>AEFI</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6563,19 +6697,30 @@
         <v>AEFI surveillance</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2021-01-22</v>
+        <v>2021-02-17</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>p8T2BE6RU60</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
+        <v>AEFI - COVID vaccine</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="C4" s="4" t="str">
+        <v>ZOhxBdiRCOG</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -6610,19 +6755,19 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>lT6Ev0gPL2L</v>
+        <v>H6mFGyr4TD2</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Map</v>
+        <v>Event report</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>Geographic distribution of AEFI cases</v>
+        <v>AEFI national level summary - last 12 months</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>r0sqJrBUsfN</v>
+        <v>vZ9iAkiJlPS</v>
       </c>
       <c r="E2" s="4" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F2" s="4" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6630,19 +6775,19 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>KEyzQOeOleH</v>
+        <v>KpmevHebldP</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>Event report</v>
+        <v>Chart</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>AEFI facility level - vaccine details</v>
+        <v>AEFI Deaths</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>RbH3H7FkyXf</v>
+        <v>dwnlX9917vw</v>
       </c>
       <c r="E3" s="5" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F3" s="5" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6650,19 +6795,19 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>sODMmX8hJOJ</v>
+        <v>TjzpPA8uOca</v>
       </c>
       <c r="B4" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>AEFI - Final sub-classification</v>
+        <v>AEFI Hospitalisations</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>mCZ4qJWLyOd</v>
+        <v>LisN5damL3D</v>
       </c>
       <c r="E4" s="4" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F4" s="4" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6670,19 +6815,19 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>j7Bvq96DWgc</v>
+        <v>lT6Ev0gPL2L</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>Chart</v>
+        <v>Map</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>AEFI - Final classification</v>
+        <v>Geographic distribution of AEFI cases</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>AVPIrEV02KP</v>
+        <v>r0sqJrBUsfN</v>
       </c>
       <c r="E5" s="5" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F5" s="5" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6690,19 +6835,19 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>TeD5eJ7a0PF</v>
+        <v>KEyzQOeOleH</v>
       </c>
       <c r="B6" s="4" t="str">
         <v>Event report</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>AEFI national level - Diagnosis</v>
+        <v>AEFI facility level - vaccine details</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>tXAcL1kR2Ty</v>
+        <v>RbH3H7FkyXf</v>
       </c>
       <c r="E6" s="4" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F6" s="4" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6710,19 +6855,19 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>pzX1HTTLJU2</v>
+        <v>sODMmX8hJOJ</v>
       </c>
       <c r="B7" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>AEFI - Serious cases</v>
+        <v>AEFI - Final sub-classification</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>SHJm39vjDVV</v>
+        <v>mCZ4qJWLyOd</v>
       </c>
       <c r="E7" s="5" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F7" s="5" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6730,19 +6875,19 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>AsmRonHtIuQ</v>
+        <v>j7Bvq96DWgc</v>
       </c>
       <c r="B8" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>AEFI Cases</v>
+        <v>AEFI - Final classification</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>Xf53H3ZGZfM</v>
+        <v>AVPIrEV02KP</v>
       </c>
       <c r="E8" s="4" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F8" s="4" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6750,19 +6895,19 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>bRZac7ysPZp</v>
+        <v>TeD5eJ7a0PF</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>Chart</v>
+        <v>Event report</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>Autopsy conducted for AEFI-associated deaths</v>
+        <v>AEFI national level - Diagnosis</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>xQehhKNuKF4</v>
+        <v>tXAcL1kR2Ty</v>
       </c>
       <c r="E9" s="5" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F9" s="5" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6770,19 +6915,19 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>qeITy0Jv5vV</v>
+        <v>pzX1HTTLJU2</v>
       </c>
       <c r="B10" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>Classification of AEFI cases by Outcome (this year)</v>
+        <v>AEFI - Serious cases</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>eWra6j3Lf0p</v>
+        <v>SHJm39vjDVV</v>
       </c>
       <c r="E10" s="4" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F10" s="4" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6790,19 +6935,19 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>qp7Ml93jnSD</v>
+        <v>AsmRonHtIuQ</v>
       </c>
       <c r="B11" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>Classification of AEFI cases by Seriousness (this year)</v>
+        <v>AEFI Cases</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>P3rhM6BHf5u</v>
+        <v>Xf53H3ZGZfM</v>
       </c>
       <c r="E11" s="5" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F11" s="5" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6810,19 +6955,19 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>saUrRYwAnKv</v>
+        <v>bRZac7ysPZp</v>
       </c>
       <c r="B12" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>AEFI cases considered for Investigation</v>
+        <v>Autopsy conducted for AEFI-associated deaths</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>CCSwqBSrR2p</v>
+        <v>xQehhKNuKF4</v>
       </c>
       <c r="E12" s="4" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F12" s="4" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6830,19 +6975,19 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>ZkbjabzBFJU</v>
+        <v>qeITy0Jv5vV</v>
       </c>
       <c r="B13" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>Annual number of AEFI cases by Gender (this year)</v>
+        <v>Classification of AEFI cases by Outcome (this year)</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v>eJoXIqWNwxI</v>
+        <v>eWra6j3Lf0p</v>
       </c>
       <c r="E13" s="5" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F13" s="5" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6850,19 +6995,19 @@
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>GKTk8X9N0WC</v>
+        <v>qp7Ml93jnSD</v>
       </c>
       <c r="B14" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>Annual number and percentage of AEFI cases by Age (this year)</v>
+        <v>Classification of AEFI cases by Seriousness (this year)</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v>X6z2ji3fWRA</v>
+        <v>P3rhM6BHf5u</v>
       </c>
       <c r="E14" s="4" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F14" s="4" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6870,19 +7015,19 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>fnm8FAWtfX4</v>
+        <v>saUrRYwAnKv</v>
       </c>
       <c r="B15" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>AEFI following DPT-Hep B vaccine (this year)</v>
+        <v>AEFI cases considered for Investigation</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v>GIcbMcTfa8T</v>
+        <v>CCSwqBSrR2p</v>
       </c>
       <c r="E15" s="5" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F15" s="5" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6890,19 +7035,19 @@
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>aGRyKvSt8hB</v>
+        <v>ZkbjabzBFJU</v>
       </c>
       <c r="B16" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>AEFI following PCV vaccine (this year, last year)</v>
+        <v>Annual number of AEFI cases by Gender (this year)</v>
       </c>
       <c r="D16" s="4" t="str">
-        <v>Bk6r4Utuwck</v>
+        <v>eJoXIqWNwxI</v>
       </c>
       <c r="E16" s="4" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F16" s="4" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6910,19 +7055,19 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>Yjz5dB94OEY</v>
+        <v>GKTk8X9N0WC</v>
       </c>
       <c r="B17" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>AEFI with IPV (this year)</v>
+        <v>Annual number and percentage of AEFI cases by Age (this year)</v>
       </c>
       <c r="D17" s="5" t="str">
-        <v>PvnePpXYHTC</v>
+        <v>X6z2ji3fWRA</v>
       </c>
       <c r="E17" s="5" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F17" s="5" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6930,19 +7075,19 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>LR2jOYXZRms</v>
+        <v>fnm8FAWtfX4</v>
       </c>
       <c r="B18" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>AEFI following Hepatitis B vaccine (this year)</v>
+        <v>AEFI following DPT-Hep B vaccine (this year)</v>
       </c>
       <c r="D18" s="4" t="str">
-        <v>KyRL3dh690L</v>
+        <v>GIcbMcTfa8T</v>
       </c>
       <c r="E18" s="4" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F18" s="4" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6950,19 +7095,19 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v>wmqeA60KPWU</v>
+        <v>aGRyKvSt8hB</v>
       </c>
       <c r="B19" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>AEFI with Pentavalent (this year)</v>
+        <v>AEFI following PCV vaccine (this year, last year)</v>
       </c>
       <c r="D19" s="5" t="str">
-        <v>rMZxwNzufiq</v>
+        <v>Bk6r4Utuwck</v>
       </c>
       <c r="E19" s="5" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F19" s="5" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6970,19 +7115,19 @@
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
-        <v>vmnEfVD29Ra</v>
+        <v>Yjz5dB94OEY</v>
       </c>
       <c r="B20" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v>AEFI following Measles,Mumps and Rubella vaccine (this year)</v>
+        <v>AEFI with IPV (this year)</v>
       </c>
       <c r="D20" s="4" t="str">
-        <v>jncagVn5QqP</v>
+        <v>PvnePpXYHTC</v>
       </c>
       <c r="E20" s="4" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F20" s="4" t="str">
         <v>Dwp14f6LzSo</v>
@@ -6990,19 +7135,19 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v>eVkbnM8lnvP</v>
+        <v>LR2jOYXZRms</v>
       </c>
       <c r="B21" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>AEFI following Polio Vaccine - Oral (OPV) Bivalent Types 1 and 3 (this year)</v>
+        <v>AEFI following Hepatitis B vaccine (this year)</v>
       </c>
       <c r="D21" s="5" t="str">
-        <v>b5K0IL6MEmn</v>
+        <v>KyRL3dh690L</v>
       </c>
       <c r="E21" s="5" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F21" s="5" t="str">
         <v>Dwp14f6LzSo</v>
@@ -7010,19 +7155,19 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="str">
-        <v>FzdMlWwP563</v>
+        <v>wmqeA60KPWU</v>
       </c>
       <c r="B22" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C22" s="4" t="str">
-        <v>AEFI following Rubella vaccine (this year)</v>
+        <v>AEFI with Pentavalent (this year)</v>
       </c>
       <c r="D22" s="4" t="str">
-        <v>ZJ9BMConhM4</v>
+        <v>rMZxwNzufiq</v>
       </c>
       <c r="E22" s="4" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F22" s="4" t="str">
         <v>Dwp14f6LzSo</v>
@@ -7030,19 +7175,19 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v>nuw6MOnmL7m</v>
+        <v>vmnEfVD29Ra</v>
       </c>
       <c r="B23" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C23" s="5" t="str">
-        <v>AEFI following BCG 0.05 vaccine (this year)</v>
+        <v>AEFI following Measles,Mumps and Rubella vaccine (this year)</v>
       </c>
       <c r="D23" s="5" t="str">
-        <v>zEw8nC0TtkU</v>
+        <v>jncagVn5QqP</v>
       </c>
       <c r="E23" s="5" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F23" s="5" t="str">
         <v>Dwp14f6LzSo</v>
@@ -7050,19 +7195,19 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v>EC56gR8oLYB</v>
+        <v>eVkbnM8lnvP</v>
       </c>
       <c r="B24" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C24" s="4" t="str">
-        <v>AEFI cases by administered vaccine</v>
+        <v>AEFI following Polio Vaccine - Oral (OPV) Bivalent Types 1 and 3 (this year)</v>
       </c>
       <c r="D24" s="4" t="str">
-        <v>qqb1OAb9ZRJ</v>
+        <v>b5K0IL6MEmn</v>
       </c>
       <c r="E24" s="4" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F24" s="4" t="str">
         <v>Dwp14f6LzSo</v>
@@ -7070,19 +7215,19 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="str">
-        <v>eFP44GxAuby</v>
+        <v>FzdMlWwP563</v>
       </c>
       <c r="B25" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C25" s="5" t="str">
-        <v>Types of AEFI reported for all Vaccines (this year)</v>
+        <v>AEFI following Rubella vaccine (this year)</v>
       </c>
       <c r="D25" s="5" t="str">
-        <v>nuJ4ZPIDUnt</v>
+        <v>ZJ9BMConhM4</v>
       </c>
       <c r="E25" s="5" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F25" s="5" t="str">
         <v>Dwp14f6LzSo</v>
@@ -7090,19 +7235,19 @@
     </row>
     <row r="26">
       <c r="A26" s="4" t="str">
-        <v>phMWM7To0lM</v>
+        <v>nuw6MOnmL7m</v>
       </c>
       <c r="B26" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C26" s="4" t="str">
-        <v>Number of AEFI Cases (last 12 months)</v>
+        <v>AEFI following BCG 0.05 vaccine (this year)</v>
       </c>
       <c r="D26" s="4" t="str">
-        <v>tjJL83WDiJJ</v>
+        <v>zEw8nC0TtkU</v>
       </c>
       <c r="E26" s="4" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F26" s="4" t="str">
         <v>Dwp14f6LzSo</v>
@@ -7110,19 +7255,19 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="str">
-        <v>zVMUVoocGtH</v>
+        <v>EC56gR8oLYB</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>Event report</v>
+        <v>Chart</v>
       </c>
       <c r="C27" s="5" t="str">
-        <v>AEFI LINE LISTING - this year</v>
+        <v>AEFI cases by administered vaccine</v>
       </c>
       <c r="D27" s="5" t="str">
-        <v>d197mIWmbQk</v>
+        <v>qqb1OAb9ZRJ</v>
       </c>
       <c r="E27" s="5" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F27" s="5" t="str">
         <v>Dwp14f6LzSo</v>
@@ -7130,96 +7275,1121 @@
     </row>
     <row r="28">
       <c r="A28" s="4" t="str">
-        <v>NRvH4fN1Uny</v>
+        <v>eFP44GxAuby</v>
       </c>
       <c r="B28" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C28" s="4" t="str">
-        <v>Time Interval between Date of Vaccination and Notification to Health System (this year)</v>
+        <v>Types of AEFI reported for all Vaccines (this year)</v>
       </c>
       <c r="D28" s="4" t="str">
-        <v>UTVqWdeEru3</v>
+        <v>nuJ4ZPIDUnt</v>
       </c>
       <c r="E28" s="4" t="str">
-        <v>2020-12-01</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F28" s="4" t="str">
-        <v>p8T2BE6RU60</v>
+        <v>Dwp14f6LzSo</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="str">
-        <v>YsgeiuWgtpJ</v>
+        <v>phMWM7To0lM</v>
       </c>
       <c r="B29" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C29" s="5" t="str">
-        <v>Time Interval between Reporting by First Level and Date of Notification to Health System (this year)</v>
+        <v>Number of AEFI Cases (last 12 months)</v>
       </c>
       <c r="D29" s="5" t="str">
-        <v>SKsWc2m8Sil</v>
+        <v>tjJL83WDiJJ</v>
       </c>
       <c r="E29" s="5" t="str">
-        <v>2020-12-01</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F29" s="5" t="str">
-        <v>p8T2BE6RU60</v>
+        <v>Dwp14f6LzSo</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="str">
-        <v>I9NvK7o0IUK</v>
+        <v>zVMUVoocGtH</v>
       </c>
       <c r="B30" s="4" t="str">
-        <v>Chart</v>
+        <v>Event report</v>
       </c>
       <c r="C30" s="4" t="str">
-        <v>Time Interval between Onset and Notification to Health System (this year)</v>
+        <v>AEFI LINE LISTING - this year</v>
       </c>
       <c r="D30" s="4" t="str">
-        <v>wN6KssUIs3Z</v>
+        <v>d197mIWmbQk</v>
       </c>
       <c r="E30" s="4" t="str">
-        <v>2020-12-01</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F30" s="4" t="str">
-        <v>p8T2BE6RU60</v>
+        <v>Dwp14f6LzSo</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="str">
-        <v>ARb6cC85Tnr</v>
+        <v/>
       </c>
       <c r="B31" s="5" t="str">
-        <v>Chart</v>
+        <v>TEXT</v>
       </c>
       <c r="C31" s="5" t="str">
-        <v>Time Interval between Date of Notification to Health System and Date of Reporting to National Level</v>
+        <v/>
       </c>
       <c r="D31" s="5" t="str">
-        <v>GOegODNP6eK</v>
+        <v>rRgzNabCohh</v>
       </c>
       <c r="E31" s="5" t="str">
-        <v>2020-12-01</v>
+        <v>2021-02-17</v>
       </c>
       <c r="F31" s="5" t="str">
         <v>p8T2BE6RU60</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="str">
+        <v>NRvH4fN1Uny</v>
+      </c>
+      <c r="B32" s="4" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C32" s="4" t="str">
+        <v>Time Interval between Date of Vaccination and Notification to Health System (this year)</v>
+      </c>
+      <c r="D32" s="4" t="str">
+        <v>UTVqWdeEru3</v>
+      </c>
+      <c r="E32" s="4" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F32" s="4" t="str">
+        <v>p8T2BE6RU60</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="str">
+        <v>YsgeiuWgtpJ</v>
+      </c>
+      <c r="B33" s="5" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C33" s="5" t="str">
+        <v>Time Interval between Reporting by First Level and Date of Notification to Health System (this year)</v>
+      </c>
+      <c r="D33" s="5" t="str">
+        <v>SKsWc2m8Sil</v>
+      </c>
+      <c r="E33" s="5" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F33" s="5" t="str">
+        <v>p8T2BE6RU60</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="str">
+        <v>I9NvK7o0IUK</v>
+      </c>
+      <c r="B34" s="4" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C34" s="4" t="str">
+        <v>Time Interval between Onset and Notification to Health System (this year)</v>
+      </c>
+      <c r="D34" s="4" t="str">
+        <v>wN6KssUIs3Z</v>
+      </c>
+      <c r="E34" s="4" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F34" s="4" t="str">
+        <v>p8T2BE6RU60</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="5" t="str">
+        <v>ARb6cC85Tnr</v>
+      </c>
+      <c r="B35" s="5" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C35" s="5" t="str">
+        <v>Time Interval between Date of Notification to Health System and Date of Reporting to National Level</v>
+      </c>
+      <c r="D35" s="5" t="str">
+        <v>GOegODNP6eK</v>
+      </c>
+      <c r="E35" s="5" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F35" s="5" t="str">
+        <v>p8T2BE6RU60</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="str">
+        <v>eDFuPQM9v8U</v>
+      </c>
+      <c r="B36" s="4" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C36" s="4" t="str">
+        <v>AEFI cases following Novavax by Patient's Province and District (this year)</v>
+      </c>
+      <c r="D36" s="4" t="str">
+        <v>TGmDprsXtTs</v>
+      </c>
+      <c r="E36" s="4" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F36" s="4" t="str">
+        <v>ZOhxBdiRCOG</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="5" t="str">
+        <v>Gz2dOS3mAiq</v>
+      </c>
+      <c r="B37" s="5" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C37" s="5" t="str">
+        <v>AEFI cases following Moderna by Patient's Province and District (this year)</v>
+      </c>
+      <c r="D37" s="5" t="str">
+        <v>R066oz9Y3Vq</v>
+      </c>
+      <c r="E37" s="5" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F37" s="5" t="str">
+        <v>ZOhxBdiRCOG</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="str">
+        <v>G7B5qhuDM0a</v>
+      </c>
+      <c r="B38" s="4" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C38" s="4" t="str">
+        <v>AEFI cases following AstraZeneca by Patient's Province and District (this year)</v>
+      </c>
+      <c r="D38" s="4" t="str">
+        <v>aTS0Dr2mdXf</v>
+      </c>
+      <c r="E38" s="4" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F38" s="4" t="str">
+        <v>ZOhxBdiRCOG</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="5" t="str">
+        <v>UnIGdvIWQ1N</v>
+      </c>
+      <c r="B39" s="5" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C39" s="5" t="str">
+        <v xml:space="preserve">Adverse events following COVID vaccination by Patient's Province and District </v>
+      </c>
+      <c r="D39" s="5" t="str">
+        <v>zXcUu4rwUYo</v>
+      </c>
+      <c r="E39" s="5" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F39" s="5" t="str">
+        <v>ZOhxBdiRCOG</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="str">
+        <v>qd6vT5pVNlB</v>
+      </c>
+      <c r="B40" s="4" t="str">
+        <v>Map</v>
+      </c>
+      <c r="C40" s="4" t="str">
+        <v>Geographic distribution of Novavax-related AEFI cases</v>
+      </c>
+      <c r="D40" s="4" t="str">
+        <v>MzvccUOi5xh</v>
+      </c>
+      <c r="E40" s="4" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F40" s="4" t="str">
+        <v>ZOhxBdiRCOG</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="5" t="str">
+        <v>KCnw54kmHc3</v>
+      </c>
+      <c r="B41" s="5" t="str">
+        <v>Map</v>
+      </c>
+      <c r="C41" s="5" t="str">
+        <v>Geographic distribution of Moderna-related AEFI cases</v>
+      </c>
+      <c r="D41" s="5" t="str">
+        <v>En9wd6a5rpU</v>
+      </c>
+      <c r="E41" s="5" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F41" s="5" t="str">
+        <v>ZOhxBdiRCOG</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="str">
+        <v>zqB888v0wb8</v>
+      </c>
+      <c r="B42" s="4" t="str">
+        <v>Map</v>
+      </c>
+      <c r="C42" s="4" t="str">
+        <v>Geographic distribution of AstraZeneca-related AEFI cases</v>
+      </c>
+      <c r="D42" s="4" t="str">
+        <v>NHlw3TvqqyA</v>
+      </c>
+      <c r="E42" s="4" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F42" s="4" t="str">
+        <v>ZOhxBdiRCOG</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="5" t="str">
+        <v>S24zyEkZ311</v>
+      </c>
+      <c r="B43" s="5" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C43" s="5" t="str">
+        <v>AstraZeneca-associated reported AEFIs</v>
+      </c>
+      <c r="D43" s="5" t="str">
+        <v>wYS5g5MaGnG</v>
+      </c>
+      <c r="E43" s="5" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F43" s="5" t="str">
+        <v>ZOhxBdiRCOG</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="str">
+        <v>C5qirWdKTbh</v>
+      </c>
+      <c r="B44" s="4" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C44" s="4" t="str">
+        <v>Moderna-associated reported AEFIs</v>
+      </c>
+      <c r="D44" s="4" t="str">
+        <v>OIpJCskaaFY</v>
+      </c>
+      <c r="E44" s="4" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F44" s="4" t="str">
+        <v>ZOhxBdiRCOG</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="5" t="str">
+        <v>byGIC7C7EdF</v>
+      </c>
+      <c r="B45" s="5" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C45" s="5" t="str">
+        <v>Novavax-associated reported AEFIs</v>
+      </c>
+      <c r="D45" s="5" t="str">
+        <v>FQUhN2oAoIg</v>
+      </c>
+      <c r="E45" s="5" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F45" s="5" t="str">
+        <v>ZOhxBdiRCOG</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="str">
+        <v>YtRNCMQS4PY</v>
+      </c>
+      <c r="B46" s="4" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C46" s="4" t="str">
+        <v>Adverse event following COVID vaccination: AstraZeneca by pregnancy and lactation status</v>
+      </c>
+      <c r="D46" s="4" t="str">
+        <v>uAOoAMTPTsW</v>
+      </c>
+      <c r="E46" s="4" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F46" s="4" t="str">
+        <v>ZOhxBdiRCOG</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="5" t="str">
+        <v>RXlC5aWvN8v</v>
+      </c>
+      <c r="B47" s="5" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C47" s="5" t="str">
+        <v>Adverse event following COVID vaccination: Moderna  by pregnancy and lactation status</v>
+      </c>
+      <c r="D47" s="5" t="str">
+        <v>fbesosZEdCa</v>
+      </c>
+      <c r="E47" s="5" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F47" s="5" t="str">
+        <v>ZOhxBdiRCOG</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="4" t="str">
+        <v>P8iSxCvY6AA</v>
+      </c>
+      <c r="B48" s="4" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C48" s="4" t="str">
+        <v>Adverse event following COVID vaccination: Novavax by pregnancy and lactation status</v>
+      </c>
+      <c r="D48" s="4" t="str">
+        <v>xlGVFXzr9sP</v>
+      </c>
+      <c r="E48" s="4" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F48" s="4" t="str">
+        <v>ZOhxBdiRCOG</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="5" t="str">
+        <v>TeD5eJ7a0PF</v>
+      </c>
+      <c r="B49" s="5" t="str">
+        <v>Event report</v>
+      </c>
+      <c r="C49" s="5" t="str">
+        <v>AEFI national level - Diagnosis</v>
+      </c>
+      <c r="D49" s="5" t="str">
+        <v>UJFtCnIGLOn</v>
+      </c>
+      <c r="E49" s="5" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F49" s="5" t="str">
+        <v>ZOhxBdiRCOG</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="4" t="str">
+        <v>L15cr5GjPYB</v>
+      </c>
+      <c r="B50" s="4" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C50" s="4" t="str">
+        <v>Adverse Events following COVID 19 : Novavax</v>
+      </c>
+      <c r="D50" s="4" t="str">
+        <v>hyB6AodGCxN</v>
+      </c>
+      <c r="E50" s="4" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F50" s="4" t="str">
+        <v>ZOhxBdiRCOG</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="5" t="str">
+        <v>Q2fs6GXaHSV</v>
+      </c>
+      <c r="B51" s="5" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C51" s="5" t="str">
+        <v>Adverse Events following COVID 19 : Moderna</v>
+      </c>
+      <c r="D51" s="5" t="str">
+        <v>WRD3KUBzovJ</v>
+      </c>
+      <c r="E51" s="5" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F51" s="5" t="str">
+        <v>ZOhxBdiRCOG</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="4" t="str">
+        <v>Lonv4dwIjk4</v>
+      </c>
+      <c r="B52" s="4" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C52" s="4" t="str">
+        <v>Adverse Events following COVID 19 : AstraZeneca</v>
+      </c>
+      <c r="D52" s="4" t="str">
+        <v>gCxa0wRhZkt</v>
+      </c>
+      <c r="E52" s="4" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="F52" s="4" t="str">
+        <v>ZOhxBdiRCOG</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="101.7109375" customWidth="1"/>
+    <col min="2" max="2" width="94.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>AEFI following PCV vaccine (this year, last year)</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <v>aGRyKvSt8hB</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>Time Interval between Date of Notification to Health System and Date of Reporting to National Level</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <v>2021-01-22</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <v>ARb6cC85Tnr</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
+        <v>AEFI Cases</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C4" s="4" t="str">
+        <v>2021-01-22</v>
+      </c>
+      <c r="D4" s="4" t="str">
+        <v>AsmRonHtIuQ</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="str">
+        <v>Autopsy conducted for AEFI-associated deaths</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <v>2021-02-15</v>
+      </c>
+      <c r="D5" s="5" t="str">
+        <v>bRZac7ysPZp</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="str">
+        <v>Novavax-associated reported AEFIs</v>
+      </c>
+      <c r="B6" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C6" s="4" t="str">
+        <v>2021-02-15</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <v>byGIC7C7EdF</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="str">
+        <v>Moderna-associated reported AEFIs</v>
+      </c>
+      <c r="B7" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <v>2021-02-15</v>
+      </c>
+      <c r="D7" s="5" t="str">
+        <v>C5qirWdKTbh</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="str">
+        <v>AEFI cases by administered vaccine</v>
+      </c>
+      <c r="B8" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C8" s="4" t="str">
+        <v>2021-02-16</v>
+      </c>
+      <c r="D8" s="4" t="str">
+        <v>EC56gR8oLYB</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="str">
+        <v>AEFI cases following Novavax by Patient's Province and District (this year)</v>
+      </c>
+      <c r="B9" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C9" s="5" t="str">
+        <v>2021-02-08</v>
+      </c>
+      <c r="D9" s="5" t="str">
+        <v>eDFuPQM9v8U</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="str">
+        <v>Types of AEFI reported for all Vaccines (this year)</v>
+      </c>
+      <c r="B10" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C10" s="4" t="str">
+        <v>2021-02-16</v>
+      </c>
+      <c r="D10" s="4" t="str">
+        <v>eFP44GxAuby</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="str">
+        <v>AEFI following Polio Vaccine - Oral (OPV) Bivalent Types 1 and 3 (this year)</v>
+      </c>
+      <c r="B11" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C11" s="5" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="D11" s="5" t="str">
+        <v>eVkbnM8lnvP</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="str">
+        <v>AEFI following DPT-Hep B vaccine (this year)</v>
+      </c>
+      <c r="B12" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C12" s="4" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="D12" s="4" t="str">
+        <v>fnm8FAWtfX4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="str">
+        <v>AEFI following Rubella vaccine (this year)</v>
+      </c>
+      <c r="B13" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C13" s="5" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="D13" s="5" t="str">
+        <v>FzdMlWwP563</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="str">
+        <v>AEFI cases following AstraZeneca by Patient's Province and District (this year)</v>
+      </c>
+      <c r="B14" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C14" s="4" t="str">
+        <v>2021-02-08</v>
+      </c>
+      <c r="D14" s="4" t="str">
+        <v>G7B5qhuDM0a</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="5" t="str">
+        <v>Annual number and percentage of AEFI cases by Age (this year)</v>
+      </c>
+      <c r="B15" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C15" s="5" t="str">
+        <v>2021-01-25</v>
+      </c>
+      <c r="D15" s="5" t="str">
+        <v>GKTk8X9N0WC</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="str">
+        <v>AEFI cases following Moderna by Patient's Province and District (this year)</v>
+      </c>
+      <c r="B16" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C16" s="4" t="str">
+        <v>2021-02-08</v>
+      </c>
+      <c r="D16" s="4" t="str">
+        <v>Gz2dOS3mAiq</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="5" t="str">
+        <v>Time Interval between Onset and Notification to Health System (this year)</v>
+      </c>
+      <c r="B17" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C17" s="5" t="str">
+        <v>2021-01-22</v>
+      </c>
+      <c r="D17" s="5" t="str">
+        <v>I9NvK7o0IUK</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="str">
+        <v>AEFI - Final classification</v>
+      </c>
+      <c r="B18" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C18" s="4" t="str">
+        <v>2021-01-22</v>
+      </c>
+      <c r="D18" s="4" t="str">
+        <v>j7Bvq96DWgc</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="str">
+        <v>AEFI Deaths</v>
+      </c>
+      <c r="B19" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C19" s="5" t="str">
+        <v>2021-01-22</v>
+      </c>
+      <c r="D19" s="5" t="str">
+        <v>KpmevHebldP</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="str">
+        <v>Adverse Events following COVID 19 : Novavax</v>
+      </c>
+      <c r="B20" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C20" s="4" t="str">
+        <v>2021-02-15</v>
+      </c>
+      <c r="D20" s="4" t="str">
+        <v>L15cr5GjPYB</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="str">
+        <v>Adverse Events following COVID 19 : AstraZeneca</v>
+      </c>
+      <c r="B21" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C21" s="5" t="str">
+        <v>2021-02-15</v>
+      </c>
+      <c r="D21" s="5" t="str">
+        <v>Lonv4dwIjk4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="str">
+        <v>AEFI following Hepatitis B vaccine (this year)</v>
+      </c>
+      <c r="B22" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C22" s="4" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="D22" s="4" t="str">
+        <v>LR2jOYXZRms</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="5" t="str">
+        <v>Time Interval between Date of Vaccination and Notification to Health System (this year)</v>
+      </c>
+      <c r="B23" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C23" s="5" t="str">
+        <v>2021-01-22</v>
+      </c>
+      <c r="D23" s="5" t="str">
+        <v>NRvH4fN1Uny</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="str">
+        <v>AEFI following BCG 0.05 vaccine (this year)</v>
+      </c>
+      <c r="B24" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C24" s="4" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="D24" s="4" t="str">
+        <v>nuw6MOnmL7m</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="5" t="str">
+        <v>Adverse event following COVID vaccination: Novavax by pregnancy and lactation status</v>
+      </c>
+      <c r="B25" s="5" t="str">
+        <v>Adverse event following COVID 19 : Novavax vaccination by pregnancy and lactation status</v>
+      </c>
+      <c r="C25" s="5" t="str">
+        <v>2021-02-16</v>
+      </c>
+      <c r="D25" s="5" t="str">
+        <v>P8iSxCvY6AA</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="str">
+        <v>Number of AEFI Cases (last 12 months)</v>
+      </c>
+      <c r="B26" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C26" s="4" t="str">
+        <v>2021-02-15</v>
+      </c>
+      <c r="D26" s="4" t="str">
+        <v>phMWM7To0lM</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="5" t="str">
+        <v>AEFI - Serious cases</v>
+      </c>
+      <c r="B27" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C27" s="5" t="str">
+        <v>2021-01-22</v>
+      </c>
+      <c r="D27" s="5" t="str">
+        <v>pzX1HTTLJU2</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="str">
+        <v>Adverse Events following COVID 19 : Moderna</v>
+      </c>
+      <c r="B28" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C28" s="4" t="str">
+        <v>2021-02-15</v>
+      </c>
+      <c r="D28" s="4" t="str">
+        <v>Q2fs6GXaHSV</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="5" t="str">
+        <v>Classification of AEFI cases by Outcome (this year)</v>
+      </c>
+      <c r="B29" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C29" s="5" t="str">
+        <v>2021-01-22</v>
+      </c>
+      <c r="D29" s="5" t="str">
+        <v>qeITy0Jv5vV</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="str">
+        <v>Classification of AEFI cases by Seriousness (this year)</v>
+      </c>
+      <c r="B30" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C30" s="4" t="str">
+        <v>2021-01-22</v>
+      </c>
+      <c r="D30" s="4" t="str">
+        <v>qp7Ml93jnSD</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="5" t="str">
+        <v>Adverse event following COVID vaccination: Moderna  by pregnancy and lactation status</v>
+      </c>
+      <c r="B31" s="5" t="str">
+        <v>Adverse event following COVID 19 : Moderna by pregnancy and lactation status</v>
+      </c>
+      <c r="C31" s="5" t="str">
+        <v>2021-02-16</v>
+      </c>
+      <c r="D31" s="5" t="str">
+        <v>RXlC5aWvN8v</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="str">
+        <v>AstraZeneca-associated reported AEFIs</v>
+      </c>
+      <c r="B32" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C32" s="4" t="str">
+        <v>2021-02-15</v>
+      </c>
+      <c r="D32" s="4" t="str">
+        <v>S24zyEkZ311</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="str">
+        <v>AEFI cases considered for Investigation</v>
+      </c>
+      <c r="B33" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C33" s="5" t="str">
+        <v>2021-02-15</v>
+      </c>
+      <c r="D33" s="5" t="str">
+        <v>saUrRYwAnKv</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="str">
+        <v>AEFI - Final sub-classification</v>
+      </c>
+      <c r="B34" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C34" s="4" t="str">
+        <v>2021-01-25</v>
+      </c>
+      <c r="D34" s="4" t="str">
+        <v>sODMmX8hJOJ</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="5" t="str">
+        <v>AEFI Hospitalisations</v>
+      </c>
+      <c r="B35" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C35" s="5" t="str">
+        <v>2021-01-22</v>
+      </c>
+      <c r="D35" s="5" t="str">
+        <v>TjzpPA8uOca</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="str">
+        <v xml:space="preserve">Adverse events following COVID vaccination by Patient's Province and District </v>
+      </c>
+      <c r="B36" s="4" t="str">
+        <v>Adverse events following COVID vaccination by Patient's Province and District (This Year)</v>
+      </c>
+      <c r="C36" s="4" t="str">
+        <v>2021-02-15</v>
+      </c>
+      <c r="D36" s="4" t="str">
+        <v>UnIGdvIWQ1N</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="5" t="str">
+        <v>AEFI following Measles,Mumps and Rubella vaccine (this year)</v>
+      </c>
+      <c r="B37" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C37" s="5" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="D37" s="5" t="str">
+        <v>vmnEfVD29Ra</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="str">
+        <v>AEFI with Pentavalent (this year)</v>
+      </c>
+      <c r="B38" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C38" s="4" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="D38" s="4" t="str">
+        <v>wmqeA60KPWU</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="5" t="str">
+        <v>AEFI with IPV (this year)</v>
+      </c>
+      <c r="B39" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C39" s="5" t="str">
+        <v>2021-02-17</v>
+      </c>
+      <c r="D39" s="5" t="str">
+        <v>Yjz5dB94OEY</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="str">
+        <v>Time Interval between Reporting by First Level and Date of Notification to Health System (this year)</v>
+      </c>
+      <c r="B40" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C40" s="4" t="str">
+        <v>2021-01-22</v>
+      </c>
+      <c r="D40" s="4" t="str">
+        <v>YsgeiuWgtpJ</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="5" t="str">
+        <v>Adverse event following COVID vaccination: AstraZeneca by pregnancy and lactation status</v>
+      </c>
+      <c r="B41" s="5" t="str">
+        <v>Adverse event following COVID 19 : AstraZeneca vaccination by pregnancy and lactation status</v>
+      </c>
+      <c r="C41" s="5" t="str">
+        <v>2021-02-16</v>
+      </c>
+      <c r="D41" s="5" t="str">
+        <v>YtRNCMQS4PY</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="str">
+        <v>Annual number of AEFI cases by Gender (this year)</v>
+      </c>
+      <c r="B42" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C42" s="4" t="str">
+        <v>2021-01-22</v>
+      </c>
+      <c r="D42" s="4" t="str">
+        <v>ZkbjabzBFJU</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="59.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -7241,7 +8411,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>AEFI following PCV vaccine (this year, last year)</v>
+        <v>Geographic distribution of Moderna-related AEFI cases</v>
       </c>
       <c r="B2" s="4" t="str">
         <v xml:space="preserve"> </v>
@@ -7250,40 +8420,40 @@
         <v>2021-02-15</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>aGRyKvSt8hB</v>
+        <v>KCnw54kmHc3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Time Interval between Date of Notification to Health System and Date of Reporting to National Level</v>
+        <v>Geographic distribution of AEFI cases</v>
       </c>
       <c r="B3" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2021-01-22</v>
+        <v>2021-02-15</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>ARb6cC85Tnr</v>
+        <v>lT6Ev0gPL2L</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>AEFI Cases</v>
+        <v>Geographic distribution of Novavax-related AEFI cases</v>
       </c>
       <c r="B4" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2021-01-22</v>
+        <v>2021-02-15</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>AsmRonHtIuQ</v>
+        <v>qd6vT5pVNlB</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>Autopsy conducted for AEFI-associated deaths</v>
+        <v>Geographic distribution of AstraZeneca-related AEFI cases</v>
       </c>
       <c r="B5" s="5" t="str">
         <v xml:space="preserve"> </v>
@@ -7292,329 +8462,21 @@
         <v>2021-02-15</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>bRZac7ysPZp</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="str">
-        <v>AEFI cases by administered vaccine</v>
-      </c>
-      <c r="B6" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C6" s="4" t="str">
-        <v>2021-02-16</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <v>EC56gR8oLYB</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="5" t="str">
-        <v>Types of AEFI reported for all Vaccines (this year)</v>
-      </c>
-      <c r="B7" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C7" s="5" t="str">
-        <v>2021-02-16</v>
-      </c>
-      <c r="D7" s="5" t="str">
-        <v>eFP44GxAuby</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="str">
-        <v>AEFI following Polio Vaccine - Oral (OPV) Bivalent Types 1 and 3 (this year)</v>
-      </c>
-      <c r="B8" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C8" s="4" t="str">
-        <v>2021-02-15</v>
-      </c>
-      <c r="D8" s="4" t="str">
-        <v>eVkbnM8lnvP</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="5" t="str">
-        <v>AEFI following DPT-Hep B vaccine (this year)</v>
-      </c>
-      <c r="B9" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C9" s="5" t="str">
-        <v>2021-02-15</v>
-      </c>
-      <c r="D9" s="5" t="str">
-        <v>fnm8FAWtfX4</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="str">
-        <v>AEFI following Rubella vaccine (this year)</v>
-      </c>
-      <c r="B10" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C10" s="4" t="str">
-        <v>2021-02-15</v>
-      </c>
-      <c r="D10" s="4" t="str">
-        <v>FzdMlWwP563</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="5" t="str">
-        <v>Annual number and percentage of AEFI cases by Age (this year)</v>
-      </c>
-      <c r="B11" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C11" s="5" t="str">
-        <v>2021-01-25</v>
-      </c>
-      <c r="D11" s="5" t="str">
-        <v>GKTk8X9N0WC</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="str">
-        <v>Time Interval between Onset and Notification to Health System (this year)</v>
-      </c>
-      <c r="B12" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C12" s="4" t="str">
-        <v>2021-01-22</v>
-      </c>
-      <c r="D12" s="4" t="str">
-        <v>I9NvK7o0IUK</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>AEFI - Final classification</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <v>2021-01-22</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <v>j7Bvq96DWgc</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>AEFI following Hepatitis B vaccine (this year)</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <v>2021-02-15</v>
-      </c>
-      <c r="D14" s="4" t="str">
-        <v>LR2jOYXZRms</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="str">
-        <v>Time Interval between Date of Vaccination and Notification to Health System (this year)</v>
-      </c>
-      <c r="B15" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C15" s="5" t="str">
-        <v>2021-01-22</v>
-      </c>
-      <c r="D15" s="5" t="str">
-        <v>NRvH4fN1Uny</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="str">
-        <v>AEFI following BCG 0.05 vaccine (this year)</v>
-      </c>
-      <c r="B16" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C16" s="4" t="str">
-        <v>2021-02-15</v>
-      </c>
-      <c r="D16" s="4" t="str">
-        <v>nuw6MOnmL7m</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="str">
-        <v>Number of AEFI Cases (last 12 months)</v>
-      </c>
-      <c r="B17" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C17" s="5" t="str">
-        <v>2021-02-15</v>
-      </c>
-      <c r="D17" s="5" t="str">
-        <v>phMWM7To0lM</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="str">
-        <v>AEFI - Serious cases</v>
-      </c>
-      <c r="B18" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C18" s="4" t="str">
-        <v>2021-01-22</v>
-      </c>
-      <c r="D18" s="4" t="str">
-        <v>pzX1HTTLJU2</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="str">
-        <v>Classification of AEFI cases by Outcome (this year)</v>
-      </c>
-      <c r="B19" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C19" s="5" t="str">
-        <v>2021-01-22</v>
-      </c>
-      <c r="D19" s="5" t="str">
-        <v>qeITy0Jv5vV</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="str">
-        <v>Classification of AEFI cases by Seriousness (this year)</v>
-      </c>
-      <c r="B20" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C20" s="4" t="str">
-        <v>2021-01-22</v>
-      </c>
-      <c r="D20" s="4" t="str">
-        <v>qp7Ml93jnSD</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="str">
-        <v>AEFI cases considered for Investigation</v>
-      </c>
-      <c r="B21" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C21" s="5" t="str">
-        <v>2021-02-15</v>
-      </c>
-      <c r="D21" s="5" t="str">
-        <v>saUrRYwAnKv</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="str">
-        <v>AEFI - Final sub-classification</v>
-      </c>
-      <c r="B22" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C22" s="4" t="str">
-        <v>2021-01-25</v>
-      </c>
-      <c r="D22" s="4" t="str">
-        <v>sODMmX8hJOJ</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="str">
-        <v>AEFI following Measles,Mumps and Rubella vaccine (this year)</v>
-      </c>
-      <c r="B23" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C23" s="5" t="str">
-        <v>2021-02-15</v>
-      </c>
-      <c r="D23" s="5" t="str">
-        <v>vmnEfVD29Ra</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="4" t="str">
-        <v>AEFI with Pentavalent (this year)</v>
-      </c>
-      <c r="B24" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C24" s="4" t="str">
-        <v>2021-02-15</v>
-      </c>
-      <c r="D24" s="4" t="str">
-        <v>wmqeA60KPWU</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="5" t="str">
-        <v>AEFI with IPV (this year)</v>
-      </c>
-      <c r="B25" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C25" s="5" t="str">
-        <v>2021-02-15</v>
-      </c>
-      <c r="D25" s="5" t="str">
-        <v>Yjz5dB94OEY</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="4" t="str">
-        <v>Time Interval between Reporting by First Level and Date of Notification to Health System (this year)</v>
-      </c>
-      <c r="B26" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C26" s="4" t="str">
-        <v>2021-01-22</v>
-      </c>
-      <c r="D26" s="4" t="str">
-        <v>YsgeiuWgtpJ</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="5" t="str">
-        <v>Annual number of AEFI cases by Gender (this year)</v>
-      </c>
-      <c r="B27" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C27" s="5" t="str">
-        <v>2021-01-22</v>
-      </c>
-      <c r="D27" s="5" t="str">
-        <v>ZkbjabzBFJU</v>
+        <v>zqB888v0wb8</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="46.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -7636,96 +8498,65 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Geographic distribution of AEFI cases</v>
+        <v>AEFI national level summary - last 12 months</v>
       </c>
       <c r="B2" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-02-15</v>
+        <v>2021-02-17</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>lT6Ev0gPL2L</v>
+        <v>H6mFGyr4TD2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>AEFI facility level - vaccine details</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <v>2021-01-28</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <v>KEyzQOeOleH</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
+        <v>AEFI national level - Diagnosis</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C4" s="4" t="str">
+        <v>2021-01-22</v>
+      </c>
+      <c r="D4" s="4" t="str">
+        <v>TeD5eJ7a0PF</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="str">
+        <v>AEFI LINE LISTING - this year</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <v>2021-02-05</v>
+      </c>
+      <c r="D5" s="5" t="str">
+        <v>zVMUVoocGtH</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
-  </sheetViews>
-  <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="str">
-        <v>Name</v>
-      </c>
-      <c r="B1" s="3" t="str">
-        <v>Description</v>
-      </c>
-      <c r="C1" s="3" t="str">
-        <v>Last updated</v>
-      </c>
-      <c r="D1" s="3" t="str">
-        <v>UID</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="str">
-        <v>AEFI facility level - vaccine details</v>
-      </c>
-      <c r="B2" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C2" s="4" t="str">
-        <v>2021-01-28</v>
-      </c>
-      <c r="D2" s="4" t="str">
-        <v>KEyzQOeOleH</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="str">
-        <v>AEFI national level - Diagnosis</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>2021-01-22</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <v>TeD5eJ7a0PF</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>AEFI LINE LISTING - this year</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>2021-02-05</v>
-      </c>
-      <c r="D4" s="4" t="str">
-        <v>zVMUVoocGtH</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -7807,7 +8638,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -7835,7 +8666,7 @@
         <v>AEFI access</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2021-02-16</v>
+        <v>2021-02-17</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>J3mFUNTreYY</v>
@@ -7857,7 +8688,7 @@
         <v>AEFI data capture</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2021-02-16</v>
+        <v>2021-02-17</v>
       </c>
       <c r="C4" s="4" t="str">
         <v>RWyhKm0cuQ5</v>
@@ -7868,7 +8699,7 @@
         <v>AEFI district</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>2021-02-16</v>
+        <v>2021-02-17</v>
       </c>
       <c r="C5" s="5" t="str">
         <v>TounOa4q45N</v>
@@ -7879,7 +8710,7 @@
         <v>AEFI first-level decision making</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2021-02-16</v>
+        <v>2021-02-17</v>
       </c>
       <c r="C6" s="4" t="str">
         <v>xgu9ZjvZRPG</v>
@@ -7890,7 +8721,7 @@
         <v>AEFI national</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>2021-02-16</v>
+        <v>2021-02-17</v>
       </c>
       <c r="C7" s="5" t="str">
         <v>YfEyw7KWMWy</v>
@@ -7900,7 +8731,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -8234,7 +9065,7 @@
         <v>Person</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-01-22</v>
+        <v>2021-02-16</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -8279,7 +9110,7 @@
         <v>Noldaaz2TLs</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-02-05T11:56:15.853</v>
+        <v>2021-02-16T17:44:58.038</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -8293,7 +9124,7 @@
         <v>so8YZ9J3MeO</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2021-01-22T14:31:15.502</v>
+        <v>2021-02-16T17:44:57.990</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>EZkN8vYZwjR</v>
@@ -8307,7 +9138,7 @@
         <v>Y4v9hBo2Xst</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2021-02-05T11:56:16.056</v>
+        <v>2021-02-16T17:44:58.041</v>
       </c>
       <c r="D4" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -9423,10 +10254,10 @@
         <v>AEFI</v>
       </c>
       <c r="B100" s="4" t="str">
-        <v>Severe events reported</v>
+        <v>Diluent 4 details</v>
       </c>
       <c r="C100" s="4" t="str">
-        <v>AEFI - Death</v>
+        <v>AEFI - Diluent 4</v>
       </c>
     </row>
     <row r="101">
@@ -9434,10 +10265,10 @@
         <v>AEFI</v>
       </c>
       <c r="B101" s="5" t="str">
-        <v>Diluent 4 details</v>
+        <v>Severe events reported</v>
       </c>
       <c r="C101" s="5" t="str">
-        <v>AEFI - Diluent 4</v>
+        <v>AEFI - Death</v>
       </c>
     </row>
     <row r="102">
@@ -9445,10 +10276,10 @@
         <v>AEFI</v>
       </c>
       <c r="B102" s="4" t="str">
-        <v/>
+        <v>Diluent 4 details</v>
       </c>
       <c r="C102" s="4" t="str">
-        <v>AEFI - Autopsy conducted</v>
+        <v>AEFI - Diluent batch/lot number 4</v>
       </c>
     </row>
     <row r="103">
@@ -9456,10 +10287,10 @@
         <v>AEFI</v>
       </c>
       <c r="B103" s="5" t="str">
-        <v>Diluent 4 details</v>
+        <v/>
       </c>
       <c r="C103" s="5" t="str">
-        <v>AEFI - Diluent batch/lot number 4</v>
+        <v>AEFI - Autopsy conducted</v>
       </c>
     </row>
     <row r="104">
@@ -9467,10 +10298,10 @@
         <v>AEFI</v>
       </c>
       <c r="B104" s="4" t="str">
-        <v>Diluent 4 details</v>
+        <v/>
       </c>
       <c r="C104" s="4" t="str">
-        <v>AEFI - Expiry date (Diluent 4)</v>
+        <v>AEFI - Lymphadenopathy</v>
       </c>
     </row>
     <row r="105">
@@ -9478,10 +10309,10 @@
         <v>AEFI</v>
       </c>
       <c r="B105" s="5" t="str">
-        <v/>
+        <v>Diluent 4 details</v>
       </c>
       <c r="C105" s="5" t="str">
-        <v>AEFI - Lymphadenopathy</v>
+        <v>AEFI - Expiry date (Diluent 4)</v>
       </c>
     </row>
     <row r="106">
@@ -9489,10 +10320,10 @@
         <v>AEFI</v>
       </c>
       <c r="B106" s="4" t="str">
-        <v/>
+        <v>Vaccine 4 details</v>
       </c>
       <c r="C106" s="4" t="str">
-        <v>AEFI - Bell's Palsy</v>
+        <v>AEFI - Expiry date (Vaccine 4)</v>
       </c>
     </row>
     <row r="107">
@@ -9500,10 +10331,10 @@
         <v>AEFI</v>
       </c>
       <c r="B107" s="5" t="str">
-        <v>Vaccine 4 details</v>
+        <v/>
       </c>
       <c r="C107" s="5" t="str">
-        <v>AEFI - Expiry date (Vaccine 4)</v>
+        <v>AEFI - Bell's Palsy</v>
       </c>
     </row>
     <row r="108">
@@ -9511,10 +10342,10 @@
         <v>AEFI</v>
       </c>
       <c r="B108" s="4" t="str">
-        <v>Vaccine 1 details</v>
+        <v/>
       </c>
       <c r="C108" s="4" t="str">
-        <v>AEFI - Vaccine 1 brand</v>
+        <v>AEFI - Is the patient pregnant?</v>
       </c>
     </row>
     <row r="109">
@@ -9522,10 +10353,10 @@
         <v>AEFI</v>
       </c>
       <c r="B109" s="5" t="str">
-        <v/>
+        <v>Vaccine 1 details</v>
       </c>
       <c r="C109" s="5" t="str">
-        <v>AEFI - Is the patient pregnant?</v>
+        <v>AEFI - Vaccine 1 brand</v>
       </c>
     </row>
     <row r="110">
@@ -16320,7 +17151,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -16470,16 +17301,16 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>f2kBCb35F4Q</v>
+        <v>EyDd8gyC4Ej</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>Hide severe local reaction type if severe local reaction is not true</v>
+        <v>Hide vaccine 4 details section if vaccine 3 has no value</v>
       </c>
       <c r="C9" s="5" t="str">
         <v/>
       </c>
       <c r="D9" s="5" t="str">
-        <v>2021-02-05</v>
+        <v>2021-02-17</v>
       </c>
       <c r="E9" s="5" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16487,16 +17318,16 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>G2OQqzZhWLo</v>
+        <v>f2kBCb35F4Q</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Hide vaccine 2 and 3 details sections if vaccine 1 has no value</v>
+        <v>Hide severe local reaction type if severe local reaction is not true</v>
       </c>
       <c r="C10" s="4" t="str">
         <v/>
       </c>
       <c r="D10" s="4" t="str">
-        <v>2021-01-31</v>
+        <v>2021-02-05</v>
       </c>
       <c r="E10" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16504,16 +17335,16 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>gng0CUI6zSW</v>
+        <v>G2OQqzZhWLo</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Final causality - B</v>
+        <v>Hide vaccine 2, 3 and 4 details sections if vaccine 1 has no value</v>
       </c>
       <c r="C11" s="5" t="str">
         <v/>
       </c>
       <c r="D11" s="5" t="str">
-        <v>2021-01-18</v>
+        <v>2021-02-17</v>
       </c>
       <c r="E11" s="5" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16521,16 +17352,16 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>gOsdoU0rUrZ</v>
+        <v>gng0CUI6zSW</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Show warning - Investigation planned date is before date of vaccination</v>
+        <v>Final causality - B</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>Show warning if nvestigation planned date is before date of vaccination</v>
+        <v/>
       </c>
       <c r="D12" s="4" t="str">
-        <v>2021-01-31</v>
+        <v>2021-01-18</v>
       </c>
       <c r="E12" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16538,13 +17369,13 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>k4VQ6HN3ViP</v>
+        <v>gOsdoU0rUrZ</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>Hide Other Vaccine (Specify)</v>
+        <v>Show warning - Investigation planned date is before date of vaccination</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v/>
+        <v>Show warning if nvestigation planned date is before date of vaccination</v>
       </c>
       <c r="D13" s="5" t="str">
         <v>2021-01-31</v>
@@ -16555,16 +17386,16 @@
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>LkxkE8r4ApM</v>
+        <v>k4VQ6HN3ViP</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>Final causality - A</v>
+        <v>Hide Other Vaccine (Specify)</v>
       </c>
       <c r="C14" s="4" t="str">
         <v/>
       </c>
       <c r="D14" s="4" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-31</v>
       </c>
       <c r="E14" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16572,16 +17403,16 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>Llp4psRq1rd</v>
+        <v>LkxkE8r4ApM</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>Hide vaccine 3 details section if vaccine 2 has no value</v>
+        <v>Final causality - A</v>
       </c>
       <c r="C15" s="5" t="str">
         <v/>
       </c>
       <c r="D15" s="5" t="str">
-        <v>2021-01-31</v>
+        <v>2021-01-18</v>
       </c>
       <c r="E15" s="5" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16589,16 +17420,16 @@
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>NegoNcSiLbL</v>
+        <v>Llp4psRq1rd</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>Hide is patient pregnant</v>
+        <v>Hide vaccine 3 details section if vaccine 2 has no value</v>
       </c>
       <c r="C16" s="4" t="str">
         <v/>
       </c>
       <c r="D16" s="4" t="str">
-        <v>2021-01-14</v>
+        <v>2021-01-31</v>
       </c>
       <c r="E16" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16606,16 +17437,16 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>nF6WxP25ZJV</v>
+        <v>NegoNcSiLbL</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>Hide Serious events</v>
+        <v>Hide is patient pregnant</v>
       </c>
       <c r="C17" s="5" t="str">
         <v/>
       </c>
       <c r="D17" s="5" t="str">
-        <v>2021-02-16</v>
+        <v>2021-01-14</v>
       </c>
       <c r="E17" s="5" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16623,16 +17454,16 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>nict9QqhO4r</v>
+        <v>nF6WxP25ZJV</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>Show warning - date of vaccination is before date of reconstitution</v>
+        <v>Hide Serious events</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>Show warning if date of vaccination is before date of reconstitution</v>
+        <v/>
       </c>
       <c r="D18" s="4" t="str">
-        <v>2021-02-05</v>
+        <v>2021-02-16</v>
       </c>
       <c r="E18" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16640,16 +17471,16 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v>nXiJZNMscRF</v>
+        <v>nict9QqhO4r</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>Final causality - Message</v>
+        <v>Show warning - date of vaccination is before date of reconstitution</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v/>
+        <v>Show warning if date of vaccination is before date of reconstitution</v>
       </c>
       <c r="D19" s="5" t="str">
-        <v>2021-01-18</v>
+        <v>2021-02-05</v>
       </c>
       <c r="E19" s="5" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16657,16 +17488,16 @@
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
-        <v>oOKWEjvSmv1</v>
+        <v>nXiJZNMscRF</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>Hide diluent  3 details section if diluent 2 has no value</v>
+        <v>Final causality - Message</v>
       </c>
       <c r="C20" s="4" t="str">
         <v/>
       </c>
       <c r="D20" s="4" t="str">
-        <v>2021-02-05</v>
+        <v>2021-01-18</v>
       </c>
       <c r="E20" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16674,16 +17505,16 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v>oWBwmPZsQVV</v>
+        <v>oOKWEjvSmv1</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>Hide Causality sub-classifications</v>
+        <v>Hide diluent  3 details section if diluent 2 has no value</v>
       </c>
       <c r="C21" s="5" t="str">
         <v/>
       </c>
       <c r="D21" s="5" t="str">
-        <v>2021-01-18</v>
+        <v>2021-02-05</v>
       </c>
       <c r="E21" s="5" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16691,16 +17522,16 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="str">
-        <v>p8T8Nfw2efM</v>
+        <v>oWBwmPZsQVV</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>Send notification when investigation needed</v>
+        <v>Hide Causality sub-classifications</v>
       </c>
       <c r="C22" s="4" t="str">
         <v/>
       </c>
       <c r="D22" s="4" t="str">
-        <v>2021-02-05</v>
+        <v>2021-01-18</v>
       </c>
       <c r="E22" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16708,16 +17539,16 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v>PKBOJnDbrKx</v>
+        <v>p8T8Nfw2efM</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>Send notification when investigation not needed and stage approved</v>
+        <v>Send notification when investigation needed</v>
       </c>
       <c r="C23" s="5" t="str">
         <v/>
       </c>
       <c r="D23" s="5" t="str">
-        <v>2021-01-31</v>
+        <v>2021-02-05</v>
       </c>
       <c r="E23" s="5" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16725,10 +17556,10 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v>r4jEt62EW64</v>
+        <v>PKBOJnDbrKx</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>Hide Other Vaccine 3 (Specify)</v>
+        <v>Send notification when investigation not needed and stage approved</v>
       </c>
       <c r="C24" s="4" t="str">
         <v/>
@@ -16742,16 +17573,16 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="str">
-        <v>tFcbiFhN3V6</v>
+        <v>r4jEt62EW64</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v>Hide Severe events section</v>
+        <v>Hide Other Vaccine 3 (Specify)</v>
       </c>
       <c r="C25" s="5" t="str">
-        <v>if severe events are not reported, hide severe events reported section</v>
+        <v/>
       </c>
       <c r="D25" s="5" t="str">
-        <v>2021-02-05</v>
+        <v>2021-01-31</v>
       </c>
       <c r="E25" s="5" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16759,16 +17590,16 @@
     </row>
     <row r="26">
       <c r="A26" s="4" t="str">
-        <v>TO0n5S5xc5D</v>
+        <v>tFcbiFhN3V6</v>
       </c>
       <c r="B26" s="4" t="str">
-        <v>Show warning - date of vaccination is before date of birth</v>
+        <v>Hide Severe events section</v>
       </c>
       <c r="C26" s="4" t="str">
-        <v>Show warning if date of vaccination is before date of birth</v>
+        <v>if severe events are not reported, hide severe events reported section</v>
       </c>
       <c r="D26" s="4" t="str">
-        <v>2021-01-31</v>
+        <v>2021-02-05</v>
       </c>
       <c r="E26" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16776,16 +17607,16 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="str">
-        <v>u3zhEvjd4gV</v>
+        <v>TO0n5S5xc5D</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>Hide diluent 2 and 3 details sections if diluent 1 has no value</v>
+        <v>Show warning - date of vaccination is before date of birth</v>
       </c>
       <c r="C27" s="5" t="str">
-        <v/>
+        <v>Show warning if date of vaccination is before date of birth</v>
       </c>
       <c r="D27" s="5" t="str">
-        <v>2021-02-05</v>
+        <v>2021-01-31</v>
       </c>
       <c r="E27" s="5" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16793,16 +17624,16 @@
     </row>
     <row r="28">
       <c r="A28" s="4" t="str">
-        <v>uCbmjtwtTLx</v>
+        <v>u3zhEvjd4gV</v>
       </c>
       <c r="B28" s="4" t="str">
-        <v>Show warning - date of reporting at national level is before date of reporting</v>
+        <v>Hide diluent 2, 3 and 4 details sections if diluent 1 has no value</v>
       </c>
       <c r="C28" s="4" t="str">
-        <v>Show warning if date of reporting at national level is before date of reporting</v>
+        <v/>
       </c>
       <c r="D28" s="4" t="str">
-        <v>2021-02-05</v>
+        <v>2021-02-17</v>
       </c>
       <c r="E28" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16810,13 +17641,13 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="str">
-        <v>uIR45kKQ8jk</v>
+        <v>uCbmjtwtTLx</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>Show warning - date of notification is before date of vaccination</v>
+        <v>Show warning - date of reporting at national level is before date of reporting</v>
       </c>
       <c r="C29" s="5" t="str">
-        <v>Show warning if date of notification is before date of vaccination</v>
+        <v>Show warning if date of reporting at national level is before date of reporting</v>
       </c>
       <c r="D29" s="5" t="str">
         <v>2021-02-05</v>
@@ -16827,16 +17658,16 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="str">
-        <v>Vgs7q2Ev5zQ</v>
+        <v>uIR45kKQ8jk</v>
       </c>
       <c r="B30" s="4" t="str">
-        <v>Hide Other Vaccine 4 (Specify)</v>
+        <v>Show warning - date of notification is before date of vaccination</v>
       </c>
       <c r="C30" s="4" t="str">
-        <v/>
+        <v>Show warning if date of notification is before date of vaccination</v>
       </c>
       <c r="D30" s="4" t="str">
-        <v>2021-01-31</v>
+        <v>2021-02-05</v>
       </c>
       <c r="E30" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16844,16 +17675,16 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="str">
-        <v>w080mrOnVjo</v>
+        <v>URrFhyvLXOU</v>
       </c>
       <c r="B31" s="5" t="str">
-        <v>Hide Other Vaccine 2 (Specify)</v>
+        <v>Hide diluent  4 details section if diluent 3 has no value</v>
       </c>
       <c r="C31" s="5" t="str">
         <v/>
       </c>
       <c r="D31" s="5" t="str">
-        <v>2021-01-31</v>
+        <v>2021-02-17</v>
       </c>
       <c r="E31" s="5" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16861,16 +17692,16 @@
     </row>
     <row r="32">
       <c r="A32" s="4" t="str">
-        <v>WgPhady3ZoS</v>
+        <v>Vgs7q2Ev5zQ</v>
       </c>
       <c r="B32" s="4" t="str">
-        <v>Hide seizure type if seizure is not true</v>
+        <v>Hide Other Vaccine 4 (Specify)</v>
       </c>
       <c r="C32" s="4" t="str">
         <v/>
       </c>
       <c r="D32" s="4" t="str">
-        <v>2021-02-05</v>
+        <v>2021-01-31</v>
       </c>
       <c r="E32" s="4" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16878,16 +17709,16 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="str">
-        <v>xUui1kMwCIR</v>
+        <v>w080mrOnVjo</v>
       </c>
       <c r="B33" s="5" t="str">
-        <v>Hide Investigation planned and investigation date</v>
+        <v>Hide Other Vaccine 2 (Specify)</v>
       </c>
       <c r="C33" s="5" t="str">
-        <v>Hide Investigation planned and investigation date when investigation is not needed in first level approval</v>
+        <v/>
       </c>
       <c r="D33" s="5" t="str">
-        <v>2021-02-05</v>
+        <v>2021-01-31</v>
       </c>
       <c r="E33" s="5" t="str">
         <v>EZkN8vYZwjR</v>
@@ -16895,18 +17726,52 @@
     </row>
     <row r="34">
       <c r="A34" s="4" t="str">
+        <v>WgPhady3ZoS</v>
+      </c>
+      <c r="B34" s="4" t="str">
+        <v>Hide seizure type if seizure is not true</v>
+      </c>
+      <c r="C34" s="4" t="str">
+        <v/>
+      </c>
+      <c r="D34" s="4" t="str">
+        <v>2021-02-05</v>
+      </c>
+      <c r="E34" s="4" t="str">
+        <v>EZkN8vYZwjR</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="5" t="str">
+        <v>xUui1kMwCIR</v>
+      </c>
+      <c r="B35" s="5" t="str">
+        <v>Hide Investigation planned and investigation date</v>
+      </c>
+      <c r="C35" s="5" t="str">
+        <v>Hide Investigation planned and investigation date when investigation is not needed in first level approval</v>
+      </c>
+      <c r="D35" s="5" t="str">
+        <v>2021-02-05</v>
+      </c>
+      <c r="E35" s="5" t="str">
+        <v>EZkN8vYZwjR</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="str">
         <v>YOik9SX7kC3</v>
       </c>
-      <c r="B34" s="4" t="str">
+      <c r="B36" s="4" t="str">
         <v>Show warning - date of death is before date of onset</v>
       </c>
-      <c r="C34" s="4" t="str">
+      <c r="C36" s="4" t="str">
         <v>Show warning if date of death is before date of onset (date AEFI started)</v>
       </c>
-      <c r="D34" s="4" t="str">
+      <c r="D36" s="4" t="str">
         <v>2021-01-31</v>
       </c>
-      <c r="E34" s="4" t="str">
+      <c r="E36" s="4" t="str">
         <v>EZkN8vYZwjR</v>
       </c>
     </row>

</xml_diff>